<commit_message>
Changed lines of code in KNET
</commit_message>
<xml_diff>
--- a/SalamtekAppiumAndroid/src/test/resources/TestData/TestDataAndroid.xlsx
+++ b/SalamtekAppiumAndroid/src/test/resources/TestData/TestDataAndroid.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="340">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -1066,6 +1066,12 @@
   </si>
   <si>
     <t>You have booked a doctor appointment with Livana Clarus Linto. The appointment number is #200010304 scheduled on 2025-11-24 at 01:15 pm.</t>
+  </si>
+  <si>
+    <t>#200010318</t>
+  </si>
+  <si>
+    <t>You have booked a doctor appointment with Livana Clarus Linto. The appointment number is #200010318 scheduled on 2025-11-26 at 12:30 pm.</t>
   </si>
 </sst>
 </file>
@@ -2232,10 +2238,10 @@
       <c r="AG4" s="0"/>
       <c r="AH4" s="0"/>
       <c r="AI4" t="s" s="0">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="AJ4" t="s" s="0">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="AK4" t="s" s="0">
         <v>292</v>

</xml_diff>

<commit_message>
Deleted all screenshots, test reports from project before push.
</commit_message>
<xml_diff>
--- a/SalamtekAppiumAndroid/src/test/resources/TestData/TestDataAndroid.xlsx
+++ b/SalamtekAppiumAndroid/src/test/resources/TestData/TestDataAndroid.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="342">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -1072,6 +1072,12 @@
   </si>
   <si>
     <t>You have booked a doctor appointment with Livana Clarus Linto. The appointment number is #200010318 scheduled on 2025-11-26 at 12:30 pm.</t>
+  </si>
+  <si>
+    <t>#200010319</t>
+  </si>
+  <si>
+    <t>You have booked a doctor appointment with Livana Clarus Linto. The appointment number is #200010319 scheduled on 2025-11-26 at 02:00 pm.</t>
   </si>
 </sst>
 </file>
@@ -2238,10 +2244,10 @@
       <c r="AG4" s="0"/>
       <c r="AH4" s="0"/>
       <c r="AI4" t="s" s="0">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="AJ4" t="s" s="0">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="AK4" t="s" s="0">
         <v>292</v>

</xml_diff>